<commit_message>
Scope and Limitations 1.2
</commit_message>
<xml_diff>
--- a/Scope_Limitations.xlsx
+++ b/Scope_Limitations.xlsx
@@ -30,9 +30,6 @@
     <t>Minimum number of concurrent users supported</t>
   </si>
   <si>
-    <t>Customers able to view all issues</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>1 second</t>
+  </si>
+  <si>
+    <t>All concurrent users see updated issue information</t>
   </si>
 </sst>
 </file>
@@ -550,10 +550,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1">
@@ -561,7 +561,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="9">
         <v>5</v>
@@ -572,10 +572,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>7</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1">
@@ -583,10 +583,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>9</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>